<commit_message>
:recycle: refactor: Refatoracao do exercicio 17
</commit_message>
<xml_diff>
--- a/out/production/linguagem-programacao--I/TesteDeMesa.xlsx
+++ b/out/production/linguagem-programacao--I/TesteDeMesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\fatec\linguagemprogramacao I\fatec-linguagem-programacaoI\tarefa 1 java\ExercicioJava\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B14C20-EE4F-4D96-AE03-F20B68FC4B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E3DE63-0DB4-410C-8D8C-26F1C832B062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" xr2:uid="{560F5334-DC9D-4D50-B0F2-1BB9E85C1802}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>Teste de Mesa Exercicios Java - Linguagem Programação I</t>
   </si>
@@ -301,9 +301,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>fator</t>
-  </si>
-  <si>
     <t>api</t>
   </si>
   <si>
@@ -316,13 +313,22 @@
     <t>3.8</t>
   </si>
   <si>
-    <t>7.8</t>
-  </si>
-  <si>
     <t>2.5</t>
   </si>
   <si>
-    <t>4.9</t>
+    <t>pontosExtras</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>7.2</t>
   </si>
 </sst>
 </file>
@@ -416,12 +422,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,8 +443,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B4C00A-5BE3-4BDE-A689-F877F31F2066}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,18 +775,19 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -782,30 +795,30 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>15</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>680</v>
       </c>
     </row>
@@ -815,48 +828,48 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>20000</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>100</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>50</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>19850</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -866,24 +879,24 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>1100</v>
       </c>
     </row>
@@ -893,10 +906,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C16" t="s">
@@ -904,10 +917,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>50000</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>86500</v>
       </c>
     </row>
@@ -917,36 +930,36 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>1000</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>10000</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>200</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>1700</v>
       </c>
     </row>
@@ -956,18 +969,18 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>100</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>37.78</v>
       </c>
     </row>
@@ -977,31 +990,31 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>5</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>11</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1009,26 +1022,26 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>10</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>-10</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1038,26 +1051,26 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>10</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>15</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>15</v>
       </c>
     </row>
@@ -1067,44 +1080,44 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>8</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>7</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>6</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>5</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1114,49 +1127,49 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>2025</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>1995</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>30</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>2025</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>2015</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>10</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -1164,60 +1177,60 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>5</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>5</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>5</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>4</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>4</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>6</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -1225,60 +1238,60 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>5</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>5</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>5</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>4</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="5"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>4</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>6</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1286,43 +1299,43 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
+      <c r="A66" s="1">
         <v>11</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>22</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
+      <c r="A67" s="1">
         <v>13</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>5</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -1330,35 +1343,35 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+      <c r="A71" s="1">
         <v>160</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>10</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>1600</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>170</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>10</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>1750</v>
       </c>
     </row>
@@ -1368,36 +1381,36 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
+      <c r="A76" s="1">
         <v>15000</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>23000</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="1">
         <v>17000</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="1">
         <v>55000</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="1">
         <v>18333.330000000002</v>
       </c>
     </row>
@@ -1407,89 +1420,118 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I79" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H79" s="2" t="s">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
+        <v>8</v>
+      </c>
+      <c r="B80" s="4">
+        <v>6</v>
+      </c>
+      <c r="C80" s="4">
+        <v>8</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I79" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
+      <c r="E80" s="4">
+        <v>1</v>
+      </c>
+      <c r="F80" s="4">
         <v>8</v>
       </c>
-      <c r="B80" s="2">
+      <c r="G80" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
+        <v>8</v>
+      </c>
+      <c r="B81" s="4">
         <v>6</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C81" s="4">
+        <v>7</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="4">
+        <v>1</v>
+      </c>
+      <c r="F81" s="4">
+        <v>3</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="4">
+        <v>5</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
+        <v>5</v>
+      </c>
+      <c r="B82" s="4">
+        <v>6</v>
+      </c>
+      <c r="C82" s="4">
+        <v>4</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E82" s="4">
+        <v>0</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="4">
         <v>8</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" s="2">
-        <v>1.69</v>
-      </c>
-      <c r="F80" s="2">
-        <v>1</v>
-      </c>
-      <c r="G80" s="2">
-        <v>8</v>
-      </c>
-      <c r="H80" s="2">
-        <v>0</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>5</v>
-      </c>
-      <c r="B81" s="2">
-        <v>6</v>
-      </c>
-      <c r="C81" s="2">
-        <v>4</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E81" s="2">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2">
-        <v>0</v>
-      </c>
-      <c r="G81" s="2">
-        <v>0</v>
-      </c>
-      <c r="H81" s="2">
-        <v>8</v>
-      </c>
-      <c r="I81" s="2" t="s">
+      <c r="I82" s="4" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>